<commit_message>
subjective question support added
</commit_message>
<xml_diff>
--- a/public/assets/tempfiles/topicUpload.xlsx
+++ b/public/assets/tempfiles/topicUpload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t xml:space="preserve">paperCode</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">subTopic</t>
   </si>
   <si>
+    <t xml:space="preserve">questMode</t>
+  </si>
+  <si>
     <t xml:space="preserve">questType</t>
   </si>
   <si>
@@ -43,10 +46,19 @@
     <t xml:space="preserve">marks</t>
   </si>
   <si>
-    <t xml:space="preserve">P2</t>
+    <t xml:space="preserve">EEF305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
   </si>
 </sst>
 </file>
@@ -152,12 +164,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -165,11 +177,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -249,10 +261,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -282,13 +294,16 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>121212</v>
+      <c r="A2" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>1</v>
@@ -297,21 +312,24 @@
         <v>0</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>40</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="G2" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="H2" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>121213</v>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>1</v>
@@ -320,19 +338,22 @@
         <v>0</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="G3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="92" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>